<commit_message>
Feat: Added percipio_email field in users table and fixed create batch API
</commit_message>
<xml_diff>
--- a/TemporaryFileStorage/CreateBatchProject.xlsx
+++ b/TemporaryFileStorage/CreateBatchProject.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Percipio_Email</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -34,6 +37,9 @@
     <t>Trainee</t>
   </si>
   <si>
+    <t>joel.raju@experionglobal.com</t>
+  </si>
+  <si>
     <t>a.nehra@experionglobal.com</t>
   </si>
   <si>
@@ -43,6 +49,9 @@
     <t>Nigin N</t>
   </si>
   <si>
+    <t>nigin.n@experionglobal.com</t>
+  </si>
+  <si>
     <t>b.aravind@experionglobal.com</t>
   </si>
   <si>
@@ -52,6 +61,9 @@
     <t>Thimna Raphel</t>
   </si>
   <si>
+    <t>thimna.raphel@experionglobal.com</t>
+  </si>
+  <si>
     <t>b.lara@experionglobal.com</t>
   </si>
   <si>
@@ -61,6 +73,9 @@
     <t>Sreejaya V S</t>
   </si>
   <si>
+    <t>sreejaya.vs@experionglobal.com</t>
+  </si>
+  <si>
     <t>bs.akshara@experionglobal.com</t>
   </si>
   <si>
@@ -70,6 +85,9 @@
     <t>Ashik George</t>
   </si>
   <si>
+    <t>ashik.george@experionglobal.com</t>
+  </si>
+  <si>
     <t>c.devadas@experionglobal.com</t>
   </si>
   <si>
@@ -79,6 +97,9 @@
     <t>Nebil V</t>
   </si>
   <si>
+    <t>nebil.v@experionglobal.com</t>
+  </si>
+  <si>
     <t>b.sreerag@experionglobal.com</t>
   </si>
   <si>
@@ -86,6 +107,9 @@
   </si>
   <si>
     <t>Elena Maria Varghese</t>
+  </si>
+  <si>
+    <t>elena.varghese@experionglobal.com</t>
   </si>
   <si>
     <t>b.meenu@experionglobal.com</t>
@@ -109,13 +133,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -154,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -169,13 +193,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,16 +500,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="32.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="41.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
@@ -504,103 +526,127 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A7" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>